<commit_message>
Various corrections / enhancements
</commit_message>
<xml_diff>
--- a/Opale/Maquette.xlsx
+++ b/Opale/Maquette.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14400" tabRatio="730" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14400" tabRatio="730" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Accueil" sheetId="1" r:id="rId1"/>
@@ -569,7 +569,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="171">
   <si>
     <t>Nom</t>
   </si>
@@ -670,9 +670,6 @@
     <t>Réseau pro.</t>
   </si>
   <si>
-    <t>Format Mois + Sem.</t>
-  </si>
-  <si>
     <t>Format 'SA' (semaines d'aménorhée)</t>
   </si>
   <si>
@@ -1076,6 +1073,15 @@
   </si>
   <si>
     <t>Saisie dépense (informatif)</t>
+  </si>
+  <si>
+    <t>Format Mois + Sem. + jours</t>
+  </si>
+  <si>
+    <t>Terme en Semaines + jours</t>
+  </si>
+  <si>
+    <t>A prendre comme premiers points des courbes</t>
   </si>
 </sst>
 </file>
@@ -1229,7 +1235,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1272,6 +1278,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1616,7 +1628,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="4"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1797,6 +1809,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="103">
@@ -2532,7 +2547,7 @@
     </row>
     <row r="4" spans="2:8">
       <c r="B4" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D4" s="37" t="s">
         <v>17</v>
@@ -2677,26 +2692,26 @@
   <sheetData>
     <row r="2" spans="2:5">
       <c r="B2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="2:5">
       <c r="B13" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="2:5">
       <c r="B15" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2734,34 +2749,34 @@
   <sheetData>
     <row r="1" spans="2:11">
       <c r="B1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" t="s">
         <v>70</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>71</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>72</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>73</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>74</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>75</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>76</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>77</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>78</v>
-      </c>
-      <c r="K1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="2" spans="2:11">
@@ -2921,14 +2936,14 @@
   <sheetData>
     <row r="2" spans="2:11">
       <c r="B2" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" spans="2:11" ht="16" thickBot="1"/>
     <row r="4" spans="2:11" ht="16" thickTop="1">
       <c r="B4" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C4" s="56"/>
       <c r="D4" s="57"/>
@@ -3004,11 +3019,11 @@
     </row>
     <row r="14" spans="2:11">
       <c r="B14" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C14" s="25"/>
       <c r="D14" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E14" s="8"/>
       <c r="I14" s="8"/>
@@ -3025,11 +3040,11 @@
     </row>
     <row r="16" spans="2:11">
       <c r="B16" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C16" s="25"/>
       <c r="D16" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E16" s="8"/>
       <c r="I16" s="8"/>
@@ -3046,11 +3061,11 @@
     </row>
     <row r="18" spans="2:11">
       <c r="B18" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C18" s="25"/>
       <c r="D18" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E18" s="8"/>
       <c r="I18" s="8"/>
@@ -3083,13 +3098,13 @@
     </row>
     <row r="22" spans="2:11" ht="16" thickTop="1">
       <c r="B22" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C22" s="56"/>
       <c r="D22" s="57"/>
       <c r="E22" s="58"/>
       <c r="G22" s="26" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H22" s="56"/>
       <c r="I22" s="57"/>
@@ -3172,15 +3187,15 @@
     </row>
     <row r="31" spans="2:11" ht="16" thickTop="1">
       <c r="B31" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C31" s="68" t="s">
         <v>115</v>
-      </c>
-      <c r="C31" s="68" t="s">
-        <v>116</v>
       </c>
       <c r="D31" s="69"/>
       <c r="E31" s="70"/>
       <c r="G31" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H31" s="56"/>
       <c r="I31" s="57"/>
@@ -3212,7 +3227,7 @@
     </row>
     <row r="35" spans="2:10" ht="16" thickTop="1">
       <c r="C35" s="68" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D35" s="69"/>
       <c r="E35" s="77"/>
@@ -3247,7 +3262,7 @@
     <row r="39" spans="2:10" ht="17" thickTop="1" thickBot="1"/>
     <row r="40" spans="2:10" ht="16" thickTop="1">
       <c r="B40" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C40" s="47"/>
       <c r="D40" s="48"/>
@@ -3291,34 +3306,34 @@
     <row r="48" spans="2:10" ht="16" thickTop="1"/>
     <row r="50" spans="2:11" ht="30">
       <c r="B50" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="C50" t="s">
         <v>121</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
         <v>122</v>
       </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
         <v>123</v>
       </c>
-      <c r="E50" t="s">
+      <c r="F50" t="s">
         <v>124</v>
-      </c>
-      <c r="F50" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="51" spans="2:11">
       <c r="B51" s="24"/>
       <c r="C51" t="s">
+        <v>96</v>
+      </c>
+      <c r="D51" t="s">
+        <v>88</v>
+      </c>
+      <c r="E51" t="s">
+        <v>105</v>
+      </c>
+      <c r="F51" t="s">
         <v>97</v>
-      </c>
-      <c r="D51" t="s">
-        <v>89</v>
-      </c>
-      <c r="E51" t="s">
-        <v>106</v>
-      </c>
-      <c r="F51" t="s">
-        <v>98</v>
       </c>
       <c r="G51" s="24"/>
       <c r="H51" s="24"/>
@@ -3329,23 +3344,23 @@
     <row r="52" spans="2:11">
       <c r="B52" s="24"/>
       <c r="F52" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="53" spans="2:11">
       <c r="B53" s="24"/>
       <c r="F53" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="54" spans="2:11">
       <c r="B54" s="24"/>
       <c r="C54" s="30" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D54" s="24"/>
       <c r="E54" s="27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F54" s="24"/>
     </row>
@@ -3410,18 +3425,18 @@
   <sheetData>
     <row r="2" spans="2:3">
       <c r="B2" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="2:3">
       <c r="B3" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -3458,42 +3473,42 @@
     </row>
     <row r="2" spans="2:8">
       <c r="B2" s="31" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D2" s="26"/>
       <c r="E2" s="24"/>
       <c r="G2" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="2:8">
       <c r="B3" s="35" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D3" s="24">
         <v>50</v>
       </c>
       <c r="E3" s="24"/>
       <c r="G3" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H3" s="5"/>
     </row>
     <row r="4" spans="2:8">
       <c r="B4" s="35" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D4" s="24">
         <v>45</v>
@@ -3502,10 +3517,10 @@
     </row>
     <row r="5" spans="2:8">
       <c r="B5" s="35" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D5" s="24">
         <v>40</v>
@@ -3514,10 +3529,10 @@
     </row>
     <row r="6" spans="2:8">
       <c r="B6" s="36" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D6" s="24">
         <v>0</v>
@@ -3526,17 +3541,17 @@
     </row>
     <row r="7" spans="2:8">
       <c r="B7" s="36" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C7" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="D7" s="34" t="s">
         <v>136</v>
-      </c>
-      <c r="D7" s="34" t="s">
-        <v>137</v>
       </c>
       <c r="E7" s="24"/>
       <c r="G7" s="27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="2:8">
@@ -3604,37 +3619,37 @@
     <row r="2" spans="1:8" ht="16" thickTop="1"/>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -3654,7 +3669,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
@@ -3662,7 +3677,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="20" thickBot="1">
       <c r="A1" s="80" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B1" s="80"/>
       <c r="C1" s="80"/>
@@ -3674,7 +3689,7 @@
     <row r="2" spans="1:7" ht="16" thickTop="1"/>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -3684,12 +3699,12 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -3729,17 +3744,17 @@
     <row r="2" spans="1:7" ht="16" thickTop="1"/>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -3877,13 +3892,13 @@
     </row>
     <row r="4" spans="2:5">
       <c r="B4" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="2:5">
       <c r="B5" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" s="5"/>
     </row>
@@ -3895,7 +3910,7 @@
     </row>
     <row r="8" spans="2:5" ht="20" thickBot="1">
       <c r="B8" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
@@ -3907,13 +3922,13 @@
         <v>0</v>
       </c>
       <c r="C10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" t="s">
         <v>50</v>
       </c>
-      <c r="D10" t="s">
-        <v>51</v>
-      </c>
       <c r="E10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="2:5">
@@ -3975,7 +3990,7 @@
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="2:11">
@@ -4120,7 +4135,7 @@
     </row>
     <row r="21" spans="2:11">
       <c r="B21" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="2:11">
@@ -4150,8 +4165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4159,6 +4174,7 @@
     <col min="2" max="2" width="20.6640625" customWidth="1"/>
     <col min="3" max="3" width="37.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.83203125" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
     <col min="10" max="10" width="30.6640625" customWidth="1"/>
   </cols>
@@ -4179,11 +4195,14 @@
         <v>29</v>
       </c>
       <c r="K2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="2:11">
       <c r="B3" s="6"/>
+      <c r="J3" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="4" spans="2:11">
       <c r="B4" s="6" t="s">
@@ -4193,124 +4212,132 @@
         <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>168</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J4" s="5"/>
     </row>
     <row r="6" spans="2:11">
       <c r="B6" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="D6" t="s">
         <v>45</v>
       </c>
-      <c r="D6" t="s">
-        <v>46</v>
+      <c r="H6" s="81" t="s">
+        <v>170</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J6" s="5"/>
       <c r="K6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="2:11">
       <c r="B7" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C7" s="5"/>
+      <c r="H7" s="81"/>
     </row>
     <row r="8" spans="2:11">
+      <c r="H8" s="81"/>
       <c r="I8" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J8" s="5"/>
       <c r="K8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="2:11">
       <c r="B9" s="6" t="s">
-        <v>48</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="H9" s="81"/>
     </row>
     <row r="10" spans="2:11">
       <c r="B10" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" s="5"/>
+      <c r="H10" s="81"/>
       <c r="I10" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J10" s="5"/>
       <c r="K10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="2:11">
       <c r="B11" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" s="5"/>
     </row>
     <row r="13" spans="2:11">
       <c r="B13" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" s="5"/>
     </row>
     <row r="15" spans="2:11">
       <c r="B15" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C15" s="5"/>
     </row>
     <row r="16" spans="2:11">
       <c r="B16" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C16" s="5"/>
     </row>
     <row r="19" spans="2:3">
       <c r="B19" s="28" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" spans="2:3">
       <c r="B22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="2:3">
       <c r="C23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="24" spans="2:3">
       <c r="C24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="2:3">
       <c r="C25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="27" spans="2:3">
       <c r="B27" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H6:H10"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15">
@@ -4359,7 +4386,7 @@
       <c r="F2" s="37"/>
       <c r="G2" s="37"/>
       <c r="I2" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J2" s="5"/>
     </row>
@@ -4368,67 +4395,67 @@
     </row>
     <row r="4" spans="2:11">
       <c r="B4" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" t="s">
         <v>56</v>
       </c>
-      <c r="D4" t="s">
-        <v>57</v>
-      </c>
       <c r="I4" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="K4" t="s">
         <v>45</v>
-      </c>
-      <c r="K4" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="5" spans="2:11">
       <c r="I5" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="2:11">
       <c r="B6" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C6" s="5"/>
     </row>
     <row r="7" spans="2:11">
       <c r="B7" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C7" s="5"/>
       <c r="I7" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="2:11">
       <c r="I8" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="2:11">
       <c r="B9" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="2:11">
       <c r="B10" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C10" s="5"/>
       <c r="I10" s="10"/>
@@ -4436,31 +4463,31 @@
     </row>
     <row r="12" spans="2:11">
       <c r="B12" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C12" s="5"/>
       <c r="I12" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J12" s="5"/>
     </row>
     <row r="14" spans="2:11">
       <c r="B14" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E14" s="15"/>
     </row>
     <row r="16" spans="2:11">
       <c r="B16" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E16" s="15"/>
     </row>
@@ -4522,98 +4549,98 @@
     </row>
     <row r="4" spans="2:10">
       <c r="B4" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" t="s">
         <v>56</v>
       </c>
-      <c r="D4" t="s">
-        <v>57</v>
-      </c>
       <c r="I4" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J4" s="5"/>
     </row>
     <row r="6" spans="2:10">
       <c r="B6" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C6" s="5"/>
       <c r="I6" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="2:10">
       <c r="B7" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C7" s="5"/>
     </row>
     <row r="8" spans="2:10">
       <c r="I8" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="2:10">
       <c r="B9" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="2:10">
       <c r="B10" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C10" s="5"/>
       <c r="I10" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="2:10">
       <c r="I11" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="2:10">
       <c r="B12" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="2:10">
       <c r="B14" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E14" s="15"/>
     </row>
     <row r="16" spans="2:10">
       <c r="B16" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E16" s="15"/>
     </row>
     <row r="19" spans="2:7" ht="17" thickBot="1">
       <c r="B19" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C19" s="16"/>
       <c r="D19" s="16"/>
@@ -4624,7 +4651,7 @@
     <row r="20" spans="2:7" ht="16" outlineLevel="1" thickTop="1"/>
     <row r="21" spans="2:7" ht="16" outlineLevel="1" thickBot="1">
       <c r="B21" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
@@ -4632,14 +4659,14 @@
     <row r="22" spans="2:7" outlineLevel="2">
       <c r="B22" s="5"/>
       <c r="C22" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="2:7" outlineLevel="2"/>
     <row r="24" spans="2:7" outlineLevel="1"/>
     <row r="25" spans="2:7" ht="16" outlineLevel="1" thickBot="1">
       <c r="B25" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C25" s="17"/>
       <c r="D25" s="17"/>
@@ -4647,14 +4674,14 @@
     <row r="26" spans="2:7" outlineLevel="2">
       <c r="B26" s="5"/>
       <c r="C26" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="2:7" outlineLevel="2"/>
     <row r="28" spans="2:7" outlineLevel="1"/>
     <row r="29" spans="2:7" ht="16" outlineLevel="1" thickBot="1">
       <c r="B29" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C29" s="17"/>
       <c r="D29" s="17"/>
@@ -4662,14 +4689,14 @@
     <row r="30" spans="2:7" outlineLevel="2">
       <c r="B30" s="5"/>
       <c r="C30" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="2:7" outlineLevel="2"/>
     <row r="32" spans="2:7" outlineLevel="1"/>
     <row r="33" spans="2:7" ht="16" outlineLevel="1" thickBot="1">
       <c r="B33" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C33" s="17"/>
       <c r="D33" s="17"/>
@@ -4677,14 +4704,14 @@
     <row r="34" spans="2:7" outlineLevel="2">
       <c r="B34" s="5"/>
       <c r="C34" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="2:7" outlineLevel="2"/>
     <row r="36" spans="2:7" outlineLevel="1"/>
     <row r="37" spans="2:7" ht="16" outlineLevel="1" thickBot="1">
       <c r="B37" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C37" s="17"/>
       <c r="D37" s="17"/>
@@ -4692,14 +4719,14 @@
     <row r="38" spans="2:7" outlineLevel="2">
       <c r="B38" s="5"/>
       <c r="C38" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="2:7" outlineLevel="2"/>
     <row r="40" spans="2:7" outlineLevel="1"/>
     <row r="41" spans="2:7" ht="17" thickBot="1">
       <c r="B41" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C41" s="16"/>
       <c r="D41" s="16"/>
@@ -4710,7 +4737,7 @@
     <row r="42" spans="2:7" ht="16" thickTop="1"/>
     <row r="43" spans="2:7" ht="16" thickBot="1">
       <c r="B43" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C43" s="17"/>
       <c r="D43" s="17"/>
@@ -4718,12 +4745,12 @@
     <row r="44" spans="2:7">
       <c r="B44" s="5"/>
       <c r="C44" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="47" spans="2:7" ht="16" thickBot="1">
       <c r="B47" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C47" s="17"/>
       <c r="D47" s="17"/>
@@ -4731,12 +4758,12 @@
     <row r="48" spans="2:7">
       <c r="B48" s="5"/>
       <c r="C48" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="51" spans="2:4" ht="16" thickBot="1">
       <c r="B51" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C51" s="17"/>
       <c r="D51" s="17"/>
@@ -4744,12 +4771,12 @@
     <row r="52" spans="2:4">
       <c r="B52" s="5"/>
       <c r="C52" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="55" spans="2:4" ht="16" thickBot="1">
       <c r="B55" s="17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C55" s="17"/>
       <c r="D55" s="17"/>
@@ -4757,12 +4784,12 @@
     <row r="56" spans="2:4">
       <c r="B56" s="5"/>
       <c r="C56" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="59" spans="2:4" ht="16" thickBot="1">
       <c r="B59" s="17" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C59" s="17"/>
       <c r="D59" s="17"/>
@@ -4770,7 +4797,7 @@
     <row r="60" spans="2:4">
       <c r="B60" s="5"/>
       <c r="C60" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -4820,36 +4847,36 @@
   <sheetData>
     <row r="2" spans="2:6">
       <c r="B2" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
     </row>
     <row r="4" spans="2:6">
       <c r="B4" s="23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="2:6">
       <c r="B5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" t="s">
         <v>89</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>90</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>91</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>92</v>
-      </c>
-      <c r="F5" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="10" spans="2:6">
       <c r="B10" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -4892,19 +4919,19 @@
   <sheetData>
     <row r="2" spans="2:11">
       <c r="B2" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="4" spans="2:11">
       <c r="B4" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D4" s="19" t="s">
         <v>97</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>98</v>
       </c>
       <c r="H4" s="19"/>
       <c r="I4" s="19"/>
@@ -4913,10 +4940,10 @@
     </row>
     <row r="5" spans="2:11">
       <c r="C5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
@@ -4925,7 +4952,7 @@
     </row>
     <row r="6" spans="2:11">
       <c r="D6" s="20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H6" s="19"/>
       <c r="I6" s="19"/>
@@ -4935,7 +4962,7 @@
     <row r="7" spans="2:11" ht="16" thickBot="1"/>
     <row r="8" spans="2:11" ht="16" thickTop="1">
       <c r="B8" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C8" s="38"/>
       <c r="D8" s="39"/>
@@ -4980,13 +5007,13 @@
     <row r="18" spans="2:11" ht="16" thickBot="1"/>
     <row r="19" spans="2:11" ht="16" thickTop="1">
       <c r="B19" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C19" s="38"/>
       <c r="D19" s="39"/>
       <c r="E19" s="40"/>
       <c r="G19" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I19" s="47"/>
       <c r="J19" s="48"/>
@@ -5052,22 +5079,22 @@
     <row r="29" spans="2:11" ht="16" thickBot="1"/>
     <row r="30" spans="2:11" ht="16" thickTop="1">
       <c r="B30" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C30" s="47"/>
       <c r="D30" s="48"/>
       <c r="E30" s="49"/>
       <c r="G30" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H30" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J30" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="2:11">
@@ -5090,10 +5117,10 @@
       <c r="D34" s="51"/>
       <c r="E34" s="52"/>
       <c r="H34" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="3:10">
@@ -5114,10 +5141,10 @@
     <row r="38" spans="3:10" ht="16" thickTop="1"/>
     <row r="39" spans="3:10">
       <c r="C39" s="27" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>